<commit_message>
added birth cohort for age group in output table shell
</commit_message>
<xml_diff>
--- a/docs/source/gbd2017_models/concept_models/vivarium_swissre_breastcancer/output_table_shell_breastcancer.xlsx
+++ b/docs/source/gbd2017_models/concept_models/vivarium_swissre_breastcancer/output_table_shell_breastcancer.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="14100" windowHeight="10275"/>
+    <workbookView xWindow="0" yWindow="900" windowWidth="14100" windowHeight="10275"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>Location</t>
   </si>
@@ -32,9 +32,6 @@
     <t>Year</t>
   </si>
   <si>
-    <t>Age</t>
-  </si>
-  <si>
     <t>Sex</t>
   </si>
   <si>
@@ -50,9 +47,6 @@
     <t>China</t>
   </si>
   <si>
-    <t>15-30</t>
-  </si>
-  <si>
     <t>Male</t>
   </si>
   <si>
@@ -65,9 +59,6 @@
     <t>…</t>
   </si>
   <si>
-    <t>30-44</t>
-  </si>
-  <si>
     <t>Female</t>
   </si>
   <si>
@@ -77,15 +68,9 @@
     <t>Alternative</t>
   </si>
   <si>
-    <t>45-69</t>
-  </si>
-  <si>
     <t>High risk with previous treatment for DCIS but not family history</t>
   </si>
   <si>
-    <t>70+</t>
-  </si>
-  <si>
     <t>Cause</t>
   </si>
   <si>
@@ -111,6 +96,24 @@
   </si>
   <si>
     <t>Number of cases detected among policyholders</t>
+  </si>
+  <si>
+    <t>Age with birth cohort</t>
+  </si>
+  <si>
+    <t>All (1900-2005)</t>
+  </si>
+  <si>
+    <t>15-30 (1990-2005)</t>
+  </si>
+  <si>
+    <t>30-44 (1975-1990)</t>
+  </si>
+  <si>
+    <t>45-69 (1950-1975)</t>
+  </si>
+  <si>
+    <t>70+ (1900-1950)</t>
   </si>
 </sst>
 </file>
@@ -451,15 +454,15 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" customWidth="1"/>
     <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="59.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
@@ -471,111 +474,111 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C3" s="2">
         <v>2020</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="G3" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="H4" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C5" s="2">
         <v>2040</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G5" s="1"/>
     </row>
@@ -584,7 +587,7 @@
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>

</xml_diff>

<commit_message>
added measure of deaths to output shell table
</commit_message>
<xml_diff>
--- a/docs/source/gbd2017_models/concept_models/vivarium_swissre_breastcancer/output_table_shell_breastcancer.xlsx
+++ b/docs/source/gbd2017_models/concept_models/vivarium_swissre_breastcancer/output_table_shell_breastcancer.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="900" windowWidth="14100" windowHeight="10275"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6825"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>Location</t>
   </si>
@@ -68,9 +68,6 @@
     <t>Alternative</t>
   </si>
   <si>
-    <t>High risk with previous treatment for DCIS but not family history</t>
-  </si>
-  <si>
     <t>Cause</t>
   </si>
   <si>
@@ -83,9 +80,6 @@
     <t>Stage 1+ breast cancer</t>
   </si>
   <si>
-    <t>Mortality &amp; morbidity (not required by client)</t>
-  </si>
-  <si>
     <t>Change of detected cases among policyholders as compared with baseline</t>
   </si>
   <si>
@@ -114,6 +108,15 @@
   </si>
   <si>
     <t>70+ (1900-1950)</t>
+  </si>
+  <si>
+    <t>High risk with previous diagnosis for DCIS or LCIS but not family history</t>
+  </si>
+  <si>
+    <t>Number of deaths from breast cancer among policyholders who did not have their breast cancer detected</t>
+  </si>
+  <si>
+    <t>Change of deaths from breast cancer among policyholders who did not have their breast cancer detected as compared with baseline</t>
   </si>
 </sst>
 </file>
@@ -453,34 +456,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" customWidth="1"/>
-    <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="59.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.3984375" customWidth="1"/>
+    <col min="4" max="4" width="21.1328125" customWidth="1"/>
+    <col min="5" max="5" width="7.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="59.1328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="68.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="106" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>2</v>
@@ -495,41 +498,41 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="2">
         <v>2020</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>7</v>
@@ -541,19 +544,19 @@
         <v>13</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>11</v>
@@ -562,41 +565,44 @@
         <v>12</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="2">
         <v>2040</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H5" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="H8" s="1"/>
     </row>
   </sheetData>

</xml_diff>